<commit_message>
Export template modify for PPT
</commit_message>
<xml_diff>
--- a/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/BubbleChart.xlsx
+++ b/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/BubbleChart.xlsx
@@ -83,14 +83,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,11 +337,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="116117440"/>
-        <c:axId val="116118016"/>
+        <c:axId val="112381888"/>
+        <c:axId val="112382464"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="116117440"/>
+        <c:axId val="112381888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -351,12 +351,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116118016"/>
+        <c:crossAx val="112382464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116118016"/>
+        <c:axId val="112382464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,7 +366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116117440"/>
+        <c:crossAx val="112381888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -395,7 +395,7 @@
         </a:ln>
       </c:spPr>
     </c:legend>
-    <c:plotVisOnly val="1"/>
+    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
@@ -414,13 +414,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>22243</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>92056</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -430,15 +430,21 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="11182350" cy="685799"/>
+          <a:off x="0" y="22243"/>
+          <a:ext cx="11182350" cy="641313"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -772,7 +778,7 @@
   <dimension ref="A4:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,70 +787,70 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
     </row>
-    <row r="30" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+    <row r="30" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>